<commit_message>
Edits to Raman section of ch6
</commit_message>
<xml_diff>
--- a/tables/ch6/threshold-shifts.xlsx
+++ b/tables/ch6/threshold-shifts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perkinne\OneDrive - Victoria University of Wellington - STAFF\Ned_Natalie_PhD\PhD-thesis\phd-thesis\tables\ch6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A09035-9135-4369-93E5-14CB877324D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D4173-0EE1-4BDF-A47C-B0EF83A1634D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="16320" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,9 +89,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +391,7 @@
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -389,67 +399,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2">
-        <f>-0.04-0.09</f>
-        <v>-0.13</v>
+        <f>-0.05-0.11</f>
+        <v>-0.16</v>
       </c>
       <c r="C2">
         <f>-0.05-0.1</f>
         <v>-0.15000000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <f>-0.08-0.11</f>
-        <v>-0.19</v>
+        <f>0.01-0.14</f>
+        <v>-0.13</v>
       </c>
       <c r="C3">
         <f>0.02-0.16</f>
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>-0.05-0.11</f>
-        <v>-0.16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <f>0.01-0.14</f>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
         <v>-0.13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <f>AVERAGE(B2:B5)</f>
-        <v>-0.1525</v>
+        <f>AVERAGE(B4:B5)</f>
+        <v>-0.16</v>
       </c>
       <c r="C6" s="1">
         <f>AVERAGE(C2:C3)</f>
         <v>-0.14500000000000002</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <f>_xlfn.STDEV.S(B2:B5)</f>
-        <v>2.8722813232690173E-2</v>
+        <f>_xlfn.STDEV.S(B5:B6)</f>
+        <v>2.1213203435596427E-2</v>
       </c>
       <c r="C7" s="1">
         <f>_xlfn.STDEV.S(C2:C3)</f>
         <v>7.0710678118654814E-3</v>
       </c>
-      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed chapter order, corrections to ch4
</commit_message>
<xml_diff>
--- a/tables/ch6/threshold-shifts.xlsx
+++ b/tables/ch6/threshold-shifts.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/treachne_staff_vuw_ac_nz/Documents/Ned_Natalie_PhD/PhD-thesis/phd-thesis/tables/ch6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perkinne\OneDrive - Victoria University of Wellington - STAFF\Ned_Natalie_PhD\PhD-thesis\phd-thesis\tables\ch6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_F25DC773A252ABDACC1048F3819E6E4C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F4D067-F501-4808-9558-5FD553BAE728}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D4173-0EE1-4BDF-A47C-B0EF83A1634D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="3525" windowWidth="15630" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Averages</t>
   </si>
@@ -50,18 +49,21 @@
   <si>
     <t>std</t>
   </si>
-  <si>
-    <t>PBASE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,9 +89,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,100 +391,72 @@
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2">
-        <f>-0.09-0.06</f>
-        <v>-0.15</v>
+        <f>-0.05-0.11</f>
+        <v>-0.16</v>
       </c>
       <c r="C2">
-        <f>-0.05-0.13</f>
-        <v>-0.18</v>
-      </c>
-      <c r="D2">
-        <f>0-0.09</f>
-        <v>-0.09</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <f>-0.05-0.1</f>
+        <v>-0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <f>-0.12-0.09</f>
-        <v>-0.21</v>
+        <f>0.01-0.14</f>
+        <v>-0.13</v>
       </c>
       <c r="C3">
-        <f>-0.07-0.08</f>
-        <v>-0.15000000000000002</v>
-      </c>
-      <c r="D3">
-        <f>0.08-0.15</f>
-        <v>-6.9999999999999993E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>-0.1-0.09</f>
+        <f>0.02-0.16</f>
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>-0.19</v>
       </c>
-      <c r="D4">
-        <f>0.08-0.16</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <f>-0.13-0.05</f>
-        <v>-0.18</v>
-      </c>
-      <c r="D5">
-        <f>0.07-0.13</f>
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <f>AVERAGE(B2:B5)</f>
-        <v>-0.1825</v>
+        <f>AVERAGE(B4:B5)</f>
+        <v>-0.16</v>
       </c>
       <c r="C6" s="1">
         <f>AVERAGE(C2:C3)</f>
-        <v>-0.16500000000000001</v>
-      </c>
-      <c r="D6" s="1">
-        <f>AVERAGE(D2:D5)</f>
-        <v>-7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.14500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <f>_xlfn.STDEV.S(B2:B5)</f>
-        <v>2.5000000000000105E-2</v>
+        <f>_xlfn.STDEV.S(B5:B6)</f>
+        <v>2.1213203435596427E-2</v>
       </c>
       <c r="C7" s="1">
         <f>_xlfn.STDEV.S(C2:C3)</f>
-        <v>2.1213203435596406E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <f>_xlfn.STDEV.S(D2:D5)</f>
-        <v>1.2909944487358016E-2</v>
+        <v>7.0710678118654814E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>